<commit_message>
MAJ fichier Word et Excel
</commit_message>
<xml_diff>
--- a/visualisation.xlsx
+++ b/visualisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\audri\Documents\Audric\Ecole\1ere année\Projet 1\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBDF4DA-566C-4180-81FC-BB2115BD870E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445CCC90-A3B3-4060-BEA5-CABD69B773DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ABF9CC3D-F386-4D28-BE6A-BD52A1FD02F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABF9CC3D-F386-4D28-BE6A-BD52A1FD02F7}"/>
   </bookViews>
   <sheets>
     <sheet name="BDD(requête sql)" sheetId="6" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Ravshan Irmatov</t>
   </si>
@@ -292,9 +292,6 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
-  <si>
-    <t>x²</t>
-  </si>
 </sst>
 </file>
 
@@ -303,7 +300,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4988,11 +4985,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2920A165-2EEF-43AE-A2EF-E066F6EC5DD8}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
@@ -5005,7 +5002,7 @@
     <col min="9" max="9" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5034,7 +5031,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5065,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5096,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5127,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5158,7 +5155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -5189,7 +5186,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5220,7 +5217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5251,7 +5248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -5282,7 +5279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -5313,7 +5310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -5344,7 +5341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -5375,7 +5372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -5406,7 +5403,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -5437,7 +5434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -5468,7 +5465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -5499,7 +5496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -5530,7 +5527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -5561,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -5592,7 +5589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -5623,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -5654,7 +5651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -5685,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -5716,7 +5713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -5747,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -5778,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -5809,7 +5806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -5840,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -5871,7 +5868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -5902,7 +5899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -5933,7 +5930,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -5964,7 +5961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -5995,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -6026,7 +6023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -6057,7 +6054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -6088,7 +6085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -6119,7 +6116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -6150,7 +6147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -6181,7 +6178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -6212,7 +6209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -6243,7 +6240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -6274,7 +6271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -6305,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -6336,7 +6333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -6367,7 +6364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -6398,7 +6395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -6429,7 +6426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -6460,7 +6457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -6491,7 +6488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -6537,18 +6534,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7911E6F-2CA0-43E0-9C42-2D74F6C1DED5}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A58" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>61</v>
       </c>
@@ -6568,7 +6565,7 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -6579,7 +6576,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -6590,7 +6587,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -6601,7 +6598,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -6612,7 +6609,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -6623,7 +6620,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -6634,12 +6631,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>52</v>
       </c>
@@ -6650,7 +6642,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -6661,7 +6653,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
@@ -6672,7 +6664,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>44</v>
       </c>
@@ -6683,7 +6675,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
@@ -6694,7 +6686,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>41</v>
       </c>
@@ -6705,7 +6697,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
@@ -6716,7 +6708,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>43</v>
       </c>
@@ -6727,7 +6719,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
@@ -6738,7 +6730,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>37</v>
       </c>
@@ -6749,7 +6741,7 @@
         <v>3.2083333333333335</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>38</v>
       </c>
@@ -6773,17 +6765,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E651D2A-6E37-4228-B008-93EAD4B0FCC6}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -6798,7 +6790,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -6806,7 +6798,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -6814,7 +6806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -6822,7 +6814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -6830,7 +6822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -6838,7 +6830,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -6846,7 +6838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -6854,7 +6846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -6862,7 +6854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
@@ -6870,7 +6862,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>65</v>
       </c>

</xml_diff>